<commit_message>
Fix missing 2050 value for GDPbES
</commit_message>
<xml_diff>
--- a/InputData/elec/GDPbES/Guaranteed Dispatch Perc by Elec Source.xlsx
+++ b/InputData/elec/GDPbES/Guaranteed Dispatch Perc by Elec Source.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\GDPbES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49048E95-F738-488C-ACC6-7107F5F38064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF73F71-0543-43DC-85EF-555AF13B1D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -621,8 +621,8 @@
   </sheetPr>
   <dimension ref="A1:AK25"/>
   <sheetViews>
-    <sheetView topLeftCell="H4" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25:AJ25"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="AK26" sqref="AK26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4050,6 +4050,9 @@
       <c r="AJ25">
         <v>0</v>
       </c>
+      <c r="AK25">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>